<commit_message>
Added 2020 and first half of 2021
</commit_message>
<xml_diff>
--- a/Conductivites_Data.xlsx
+++ b/Conductivites_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthiasgolomb/Box/Results/MOFs/ConductivityChart/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthiasgolomb/Documents/GitHub/ConductivityChart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D5EB17A-F3F5-6A4B-8AEB-E5976E456ED6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3047FD-C4DC-3A4B-96A4-B3EE09E36E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{FA4547AC-B233-9C41-8F1C-4177ED449BD6}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{FA4547AC-B233-9C41-8F1C-4177ED449BD6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -174,6 +174,39 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>10.1002/adfm.202007294</t>
+  </si>
+  <si>
+    <t>Cu(H2O)(2,6-NDPA)0.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1002/anie.201912642 </t>
+  </si>
+  <si>
+    <t>Cu-BDC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1038/s41557-019-0372-0 </t>
+  </si>
+  <si>
+    <t>HoHTTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1038/s41557-021-00666-6 </t>
+  </si>
+  <si>
+    <t>Cr(tri)2(CF3SO3)0.33</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Fe-HHTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1002/anie.202102670 </t>
   </si>
 </sst>
 </file>
@@ -537,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9B93FB-1713-AB49-BBD4-53A468A75EB5}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="G47" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -587,7 +620,7 @@
         <v>248</v>
       </c>
       <c r="D2" s="2" t="str">
-        <f>IF(C2&gt;100,"Yes","No")</f>
+        <f t="shared" ref="D2:D12" si="0">IF(C2&gt;100,"Yes","No")</f>
         <v>Yes</v>
       </c>
       <c r="E2">
@@ -608,7 +641,7 @@
         <v>54</v>
       </c>
       <c r="D3" s="2" t="str">
-        <f>IF(C3&gt;100,"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>No</v>
       </c>
       <c r="E3">
@@ -629,7 +662,7 @@
         <v>370</v>
       </c>
       <c r="D4" s="2" t="str">
-        <f>IF(C4&gt;100,"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
       <c r="E4">
@@ -650,7 +683,7 @@
         <v>450</v>
       </c>
       <c r="D5" s="2" t="str">
-        <f>IF(C5&gt;100,"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
       <c r="E5">
@@ -671,13 +704,13 @@
         <v>50</v>
       </c>
       <c r="D6" s="2" t="str">
-        <f>IF(C6&gt;100,"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>No</v>
       </c>
       <c r="E6">
         <v>2018</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>0.3</v>
       </c>
     </row>
@@ -692,7 +725,7 @@
         <v>614</v>
       </c>
       <c r="D7" s="2" t="str">
-        <f>IF(C7&gt;100,"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
       <c r="E7">
@@ -713,7 +746,7 @@
         <v>1230</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f>IF(C8&gt;100,"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
       <c r="E8">
@@ -734,7 +767,7 @@
         <v>610</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f>IF(C9&gt;100,"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
       <c r="E9">
@@ -755,7 +788,7 @@
         <v>3</v>
       </c>
       <c r="D10" s="2" t="str">
-        <f>IF(C10&gt;100,"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>No</v>
       </c>
       <c r="E10">
@@ -773,7 +806,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="2" t="str">
-        <f>IF(C11&gt;100,"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>No</v>
       </c>
       <c r="E11">
@@ -794,7 +827,7 @@
         <v>1175</v>
       </c>
       <c r="D12" s="2" t="str">
-        <f>IF(C12&gt;100,"Yes","No")</f>
+        <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
       <c r="E12">
@@ -1301,11 +1334,123 @@
       <c r="E38">
         <v>2020</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="2">
         <v>11.5</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D39" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39">
+        <v>2020</v>
+      </c>
+      <c r="F39" s="2">
+        <v>2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>271</v>
+      </c>
+      <c r="D40" t="s">
+        <v>46</v>
+      </c>
+      <c r="E40">
+        <v>2020</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="G40" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>52</v>
+      </c>
+      <c r="B41" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41">
+        <v>208</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41">
+        <v>2020</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="G41" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42">
+        <v>80</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E42">
+        <v>2021</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G42" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>56</v>
+      </c>
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43">
+        <v>1400</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E43">
+        <v>2021</v>
+      </c>
+      <c r="F43" s="2">
+        <v>1E-3</v>
+      </c>
+      <c r="G43" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added 2D layered MOF from 2021
</commit_message>
<xml_diff>
--- a/Conductivites_Data.xlsx
+++ b/Conductivites_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthiasgolomb/Documents/GitHub/ConductivityChart/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3047FD-C4DC-3A4B-96A4-B3EE09E36E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67F99A28-203C-844C-8147-E9776712A18C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{FA4547AC-B233-9C41-8F1C-4177ED449BD6}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -207,6 +207,12 @@
   </si>
   <si>
     <t xml:space="preserve">10.1002/anie.202102670 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.1021/acsaem.0c02758 </t>
+  </si>
+  <si>
+    <t>Ni3(HAB)2</t>
   </si>
 </sst>
 </file>
@@ -570,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC9B93FB-1713-AB49-BBD4-53A468A75EB5}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G47" sqref="G47"/>
+    <sheetView tabSelected="1" topLeftCell="B12" workbookViewId="0">
+      <selection activeCell="G44" sqref="G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1453,6 +1459,29 @@
         <v>57</v>
       </c>
     </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" t="s">
+        <v>14</v>
+      </c>
+      <c r="C44">
+        <v>133</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E44">
+        <v>2021</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="G44" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G38" r:id="rId1" tooltip="Persistent link using digital object identifier" display="https://doi.org/10.1016/j.apcatb.2020.119295" xr:uid="{24DED032-023F-0D46-A810-55E26F992CF0}"/>

</xml_diff>